<commit_message>
create data entry spreadsheets for viz census, predation, ulva, viz census
</commit_message>
<xml_diff>
--- a/corals/final_spreadsheets/coral_reef_habitats_data_entry_spreadsheet_marinegeo.xlsx
+++ b/corals/final_spreadsheets/coral_reef_habitats_data_entry_spreadsheet_marinegeo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>definition</t>
   </si>
@@ -144,19 +144,25 @@
     <t xml:space="preserve">coral_demographics_notes</t>
   </si>
   <si>
+    <t xml:space="preserve">data_collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name(s) of data collector(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample metadata</t>
+  </si>
+  <si>
     <t xml:space="preserve">data_entry_person</t>
   </si>
   <si>
     <t xml:space="preserve">Full name of data entry person</t>
   </si>
   <si>
-    <t xml:space="preserve">sample metadata</t>
-  </si>
-  <si>
     <t xml:space="preserve">distance_completed_m</t>
   </si>
   <si>
-    <t xml:space="preserve">The surveyed length of the transect</t>
+    <t xml:space="preserve">The length of the transect surveyed by the data collector</t>
   </si>
   <si>
     <t xml:space="preserve">meters</t>
@@ -1098,30 +1104,30 @@
         <v>38</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
@@ -1132,14 +1138,12 @@
         <v>43</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
@@ -1147,15 +1151,17 @@
         <v>44</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F17" s="10" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
@@ -1163,15 +1169,15 @@
         <v>46</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
@@ -1198,30 +1204,28 @@
         <v>51</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22">
@@ -1253,9 +1257,11 @@
         <v>13</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F23" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
@@ -1266,12 +1272,12 @@
         <v>60</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -1282,7 +1288,7 @@
         <v>62</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -1303,7 +1309,7 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27">
@@ -1314,12 +1320,12 @@
         <v>66</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28">
@@ -1327,7 +1333,7 @@
         <v>67</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>29</v>
@@ -1335,77 +1341,77 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33">
@@ -1421,7 +1427,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
@@ -1434,30 +1440,28 @@
       <c r="C34" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="10" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36">
@@ -1471,18 +1475,36 @@
         <v>13</v>
       </c>
       <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="E36" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F36" s="10" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="A37" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1520,38 +1542,42 @@
     <col min="4" max="4" width="22.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="20.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="17.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="21.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="14.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="20.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="17.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="21.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>77</v>
+      <c r="J1" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1590,34 +1616,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="H1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>21</v>
@@ -1632,13 +1658,13 @@
         <v>19</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R1" s="12" t="s">
         <v>33</v>
@@ -1678,49 +1704,49 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>27</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>31</v>
@@ -1754,34 +1780,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>23</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>